<commit_message>
Freeze STEP 1B acceptance: CAP-001 fix + all gates pass
Changes:
- Fix CAP-001 metadata: role→observe, mutability→read (explicit in registry)
- Update STEP 0B script to use explicit fields when present
- Re-run full pipeline: STEP 0B → STEP 1 → STEP 1B → STEP 1B-R

Gate Results (FINAL):
- G1: PASS (100% baseline dominance)
- G2: PASS (CAP-001 → L21-EVD-R in all domains)
- G3: PASS (0 authority violations)
- G4: PASS (0% generation needed)

STEP 1B acceptance is now FROZEN per PIN-363.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/capabilities/applicability/capability_applicability_matrix.xlsx
+++ b/docs/capabilities/applicability/capability_applicability_matrix.xlsx
@@ -503,12 +503,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CAP-001</t>
+          <t>CAP-011</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Execution Replay &amp; Activity</t>
+          <t>M28 Governance Orchestration</t>
         </is>
       </c>
       <c r="D2" t="b">
@@ -520,16 +520,16 @@
         </is>
       </c>
       <c r="F2" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ACT-Q6</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>ACT-Q5, ACT-Q6</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
       <c r="I2" t="inlineStr">
         <is>
           <t>HIGH</t>
@@ -537,7 +537,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>CUSTOMER</t>
+          <t>FOUNDER</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Primary:4 Secondary:2 Questions:2</t>
+          <t>Primary:2 Secondary:0 Questions:1</t>
         </is>
       </c>
     </row>
@@ -559,12 +559,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CAP-011</t>
+          <t>CAP-016</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>M28 Governance Orchestration</t>
+          <t>Skill System (M2/M3)</t>
         </is>
       </c>
       <c r="D3" t="b">
@@ -593,7 +593,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>FOUNDER</t>
+          <t>SDK</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Primary:2 Secondary:0 Questions:1</t>
+          <t>Primary:2 Secondary:2 Questions:1</t>
         </is>
       </c>
     </row>
@@ -615,12 +615,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CAP-016</t>
+          <t>CAP-002</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Skill System (M2/M3)</t>
+          <t>Cost Simulation V2</t>
         </is>
       </c>
       <c r="D4" t="b">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>SDK</t>
+          <t>CUSTOMER</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Primary:2 Secondary:2 Questions:1</t>
+          <t>Primary:1 Secondary:1 Questions:1</t>
         </is>
       </c>
     </row>
@@ -671,12 +671,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CAP-002</t>
+          <t>CAP-008</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cost Simulation V2</t>
+          <t>M12 Multi-Agent Orchestration</t>
         </is>
       </c>
       <c r="D5" t="b">
@@ -700,12 +700,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>MEDIUM</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>CUSTOMER</t>
+          <t>SDK</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Primary:1 Secondary:1 Questions:1</t>
+          <t>Primary:2 Secondary:0 Questions:1</t>
         </is>
       </c>
     </row>
@@ -727,12 +727,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CAP-008</t>
+          <t>CAP-012</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>M12 Multi-Agent Orchestration</t>
+          <t>M4 Workflow Engine</t>
         </is>
       </c>
       <c r="D6" t="b">
@@ -761,7 +761,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>SDK</t>
+          <t>NONE</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -783,12 +783,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CAP-012</t>
+          <t>CAP-020</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>M4 Workflow Engine</t>
+          <t>CLI Execution</t>
         </is>
       </c>
       <c r="D7" t="b">
@@ -839,12 +839,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CAP-020</t>
+          <t>CAP-021</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CLI Execution</t>
+          <t>SDK Execution</t>
         </is>
       </c>
       <c r="D8" t="b">
@@ -868,7 +868,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>MEDIUM</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Primary:2 Secondary:0 Questions:1</t>
+          <t>Primary:1 Secondary:0 Questions:1</t>
         </is>
       </c>
     </row>
@@ -895,12 +895,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CAP-021</t>
+          <t>CAP-001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SDK Execution</t>
+          <t>Execution Replay &amp; Activity</t>
         </is>
       </c>
       <c r="D9" t="b">
@@ -912,24 +912,24 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>ACT-Q6</t>
+          <t>ACT-Q5, ACT-Q6</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>MEDIUM</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>CUSTOMER</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Primary:1 Secondary:0 Questions:1</t>
+          <t>Primary:4 Secondary:2 Questions:2</t>
         </is>
       </c>
     </row>
@@ -2679,12 +2679,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>CAP-001</t>
+          <t>CAP-002</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Execution Replay &amp; Activity</t>
+          <t>Cost Simulation V2</t>
         </is>
       </c>
       <c r="D43" t="b">
@@ -2723,7 +2723,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Primary:2 Secondary:0 Questions:3</t>
+          <t>Primary:1 Secondary:0 Questions:3</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CAP-002</t>
+          <t>CAP-005</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Cost Simulation V2</t>
+          <t>Founder Console</t>
         </is>
       </c>
       <c r="D44" t="b">
@@ -2752,16 +2752,16 @@
         </is>
       </c>
       <c r="F44" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>INC-Q5</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
         <v>1</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>INC-Q1, INC-Q2, INC-Q5</t>
-        </is>
-      </c>
-      <c r="H44" t="n">
-        <v>3</v>
-      </c>
       <c r="I44" t="inlineStr">
         <is>
           <t>HIGH</t>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>CUSTOMER</t>
+          <t>FOUNDER</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -2779,7 +2779,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Primary:1 Secondary:0 Questions:3</t>
+          <t>Primary:1 Secondary:1 Questions:1</t>
         </is>
       </c>
     </row>
@@ -2791,12 +2791,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>CAP-005</t>
+          <t>CAP-009</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Founder Console</t>
+          <t>M19 Policy Engine</t>
         </is>
       </c>
       <c r="D45" t="b">
@@ -2812,7 +2812,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>INC-Q5</t>
+          <t>INC-Q1</t>
         </is>
       </c>
       <c r="H45" t="n">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>FOUNDER</t>
+          <t>CUSTOMER</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -2835,7 +2835,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Primary:1 Secondary:1 Questions:1</t>
+          <t>Primary:0 Secondary:0 Questions:1</t>
         </is>
       </c>
     </row>
@@ -2847,12 +2847,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>CAP-009</t>
+          <t>CAP-021</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>M19 Policy Engine</t>
+          <t>SDK Execution</t>
         </is>
       </c>
       <c r="D46" t="b">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>INC-Q1</t>
+          <t>INC-Q5</t>
         </is>
       </c>
       <c r="H46" t="n">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>CUSTOMER</t>
+          <t>NONE</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -2891,7 +2891,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Primary:0 Secondary:0 Questions:1</t>
+          <t>Primary:1 Secondary:0 Questions:1</t>
         </is>
       </c>
     </row>
@@ -2903,12 +2903,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>CAP-021</t>
+          <t>CAP-001</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SDK Execution</t>
+          <t>Execution Replay &amp; Activity</t>
         </is>
       </c>
       <c r="D47" t="b">
@@ -2920,24 +2920,24 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>INC-Q5</t>
+          <t>INC-Q1, INC-Q2, INC-Q5</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>MEDIUM</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>CUSTOMER</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Primary:1 Secondary:0 Questions:1</t>
+          <t>Primary:2 Secondary:0 Questions:3</t>
         </is>
       </c>
     </row>
@@ -4831,12 +4831,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>CAP-001</t>
+          <t>CAP-002</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Execution Replay &amp; Activity</t>
+          <t>Cost Simulation V2</t>
         </is>
       </c>
       <c r="D84" t="b">
@@ -4848,16 +4848,16 @@
         </is>
       </c>
       <c r="F84" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>LOG-Q1</t>
+        </is>
+      </c>
+      <c r="H84" t="n">
         <v>1</v>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>LOG-Q1, LOG-Q2</t>
-        </is>
-      </c>
-      <c r="H84" t="n">
-        <v>2</v>
-      </c>
       <c r="I84" t="inlineStr">
         <is>
           <t>HIGH</t>
@@ -4875,7 +4875,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Primary:2 Secondary:1 Questions:2</t>
+          <t>Primary:0 Secondary:0 Questions:1</t>
         </is>
       </c>
     </row>
@@ -4887,12 +4887,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>CAP-002</t>
+          <t>CAP-021</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Cost Simulation V2</t>
+          <t>SDK Execution</t>
         </is>
       </c>
       <c r="D85" t="b">
@@ -4921,7 +4921,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>CUSTOMER</t>
+          <t>NONE</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -4943,12 +4943,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>CAP-021</t>
+          <t>CAP-001</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>SDK Execution</t>
+          <t>Execution Replay &amp; Activity</t>
         </is>
       </c>
       <c r="D86" t="b">
@@ -4960,24 +4960,24 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>0.85</v>
+        <v>0.8</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>LOG-Q1</t>
+          <t>LOG-Q1, LOG-Q2</t>
         </is>
       </c>
       <c r="H86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>MEDIUM</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>CUSTOMER</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -4987,7 +4987,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Primary:0 Secondary:0 Questions:1</t>
+          <t>Primary:2 Secondary:1 Questions:2</t>
         </is>
       </c>
     </row>
@@ -7035,12 +7035,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>CAP-001</t>
+          <t>CAP-005</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Execution Replay &amp; Activity</t>
+          <t>Founder Console</t>
         </is>
       </c>
       <c r="D126" t="b">
@@ -7056,7 +7056,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>POL-Q2</t>
+          <t>POL-Q4</t>
         </is>
       </c>
       <c r="H126" t="n">
@@ -7069,7 +7069,7 @@
       </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>CUSTOMER</t>
+          <t>FOUNDER</t>
         </is>
       </c>
       <c r="K126" t="inlineStr">
@@ -7091,12 +7091,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>CAP-005</t>
+          <t>CAP-011</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Founder Console</t>
+          <t>M28 Governance Orchestration</t>
         </is>
       </c>
       <c r="D127" t="b">
@@ -7108,15 +7108,11 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>POL-Q4</t>
-        </is>
-      </c>
+        <v>0.7</v>
+      </c>
+      <c r="G127" t="inlineStr"/>
       <c r="H127" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I127" t="inlineStr">
         <is>
@@ -7135,7 +7131,7 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>Primary:0 Secondary:0 Questions:1</t>
+          <t>Primary:1 Secondary:0 Questions:0</t>
         </is>
       </c>
     </row>
@@ -7147,12 +7143,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>CAP-011</t>
+          <t>CAP-003</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>M28 Governance Orchestration</t>
+          <t>Policy Proposals</t>
         </is>
       </c>
       <c r="D128" t="b">
@@ -7164,20 +7160,24 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="G128" t="inlineStr"/>
+        <v>0.65</v>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>POL-Q4</t>
+        </is>
+      </c>
       <c r="H128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>MEDIUM</t>
         </is>
       </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>FOUNDER</t>
+          <t>CUSTOMER</t>
         </is>
       </c>
       <c r="K128" t="inlineStr">
@@ -7187,7 +7187,7 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>Primary:1 Secondary:0 Questions:0</t>
+          <t>Primary:1 Secondary:2 Questions:1</t>
         </is>
       </c>
     </row>
@@ -7199,12 +7199,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>CAP-003</t>
+          <t>CAP-016</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Policy Proposals</t>
+          <t>Skill System (M2/M3)</t>
         </is>
       </c>
       <c r="D129" t="b">
@@ -7228,12 +7228,12 @@
       </c>
       <c r="I129" t="inlineStr">
         <is>
-          <t>MEDIUM</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>CUSTOMER</t>
+          <t>SDK</t>
         </is>
       </c>
       <c r="K129" t="inlineStr">
@@ -7243,7 +7243,7 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>Primary:1 Secondary:2 Questions:1</t>
+          <t>Primary:1 Secondary:1 Questions:1</t>
         </is>
       </c>
     </row>
@@ -7255,12 +7255,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>CAP-016</t>
+          <t>CAP-001</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Skill System (M2/M3)</t>
+          <t>Execution Replay &amp; Activity</t>
         </is>
       </c>
       <c r="D130" t="b">
@@ -7268,15 +7268,15 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>CONSUME</t>
+          <t>DEFER</t>
         </is>
       </c>
       <c r="F130" t="n">
-        <v>0.65</v>
+        <v>0.55</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>POL-Q4</t>
+          <t>POL-Q2</t>
         </is>
       </c>
       <c r="H130" t="n">
@@ -7284,12 +7284,12 @@
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>MEDIUM</t>
         </is>
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>SDK</t>
+          <t>CUSTOMER</t>
         </is>
       </c>
       <c r="K130" t="inlineStr">
@@ -7299,7 +7299,7 @@
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>Primary:1 Secondary:1 Questions:1</t>
+          <t>Low confidence. Primary:0 Secondary:0</t>
         </is>
       </c>
     </row>

</xml_diff>